<commit_message>
Änderungen Frontend CSS ordner etc.
</commit_message>
<xml_diff>
--- a/Gespraechsprotokolle/Protokoll.xlsx
+++ b/Gespraechsprotokolle/Protokoll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dreim\Git\zero1one\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dreim\Git\zero1one\Gespraechsprotokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6921F24-3CA1-427E-B5A3-14FDD32695B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99B97FF-2BBF-4F47-AF1E-094EC7654A40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Details " sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -199,6 +199,12 @@
 - https://www.youtube.com/watch?v=URf1YcifgTU&amp;ab_channel=CodingMarket
  Seiten :  Profil ; CI-Typen; CI-Record 
 </t>
+  </si>
+  <si>
+    <t>Qualitätskontrolle</t>
+  </si>
+  <si>
+    <t>Pascal Jung</t>
   </si>
 </sst>
 </file>
@@ -659,8 +665,8 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,11 +909,21 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44109</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
@@ -1130,6 +1146,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F1971A0B5C609B4AADBB87F7A9AC2B43" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2845366aab18a6db5ff4ac0a5e2925fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d413257cd9829394d17656a545d5fa4e">
     <xsd:element name="properties">
@@ -1243,33 +1274,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1773DF2-1D83-4C9F-B4DF-BF076FDEDE78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF03183-3898-4C72-A4AA-5B7883107B56}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1290,9 +1298,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF03183-3898-4C72-A4AA-5B7883107B56}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1773DF2-1D83-4C9F-B4DF-BF076FDEDE78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>